<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-27.xlsx - 2026-01-27T14:10:00.075Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-27.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-27.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,37 +449,37 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-26 12:02</v>
+        <v>2026-01-27 14:09</v>
       </c>
       <c r="C2" t="str">
-        <v>Minakshi</v>
+        <v>Girija Lakade</v>
       </c>
       <c r="D2" t="str">
-        <v>A201</v>
+        <v>A 1507</v>
       </c>
       <c r="E2" t="str">
-        <v>7387851735</v>
+        <v>74996684</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x5</v>
+        <v>Jawar Bhakari x4</v>
       </c>
       <c r="G2">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H2" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-26</v>
+        <v/>
       </c>
       <c r="K2" t="str">
-        <v>19:30</v>
+        <v/>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,37 +493,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-26 11:12</v>
+        <v>2026-01-26 12:02</v>
       </c>
       <c r="C3" t="str">
-        <v>Priyanka Patil</v>
+        <v>Minakshi</v>
       </c>
       <c r="D3" t="str">
-        <v>A-1605</v>
+        <v>A201</v>
       </c>
       <c r="E3" t="str">
-        <v>9867003224</v>
+        <v>7387851735</v>
       </c>
       <c r="F3" t="str">
-        <v>Jawar Bhakari x2</v>
+        <v>Wheat Chapati x5</v>
       </c>
       <c r="G3">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I3" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-27</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K3" t="str">
-        <v>09:00</v>
+        <v>19:30</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -537,37 +537,37 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-21 10:01</v>
+        <v>2026-01-26 11:12</v>
       </c>
       <c r="C4" t="str">
-        <v>Vipula Thakkar</v>
+        <v>Priyanka Patil</v>
       </c>
       <c r="D4" t="str">
-        <v>B-903, Kakkad lavida</v>
+        <v>A-1605</v>
       </c>
       <c r="E4" t="str">
-        <v>8109861246</v>
+        <v>9867003224</v>
       </c>
       <c r="F4" t="str">
-        <v>Appe Chutney x1</v>
+        <v>Jawar Bhakari x2</v>
       </c>
       <c r="G4">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="H4" t="str">
-        <v>DELIVERED</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-27</v>
       </c>
       <c r="K4" t="str">
-        <v/>
+        <v>09:00</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-21 07:49</v>
+        <v>2026-01-21 10:01</v>
       </c>
       <c r="C5" t="str">
-        <v>Renu</v>
+        <v>Vipula Thakkar</v>
       </c>
       <c r="D5" t="str">
-        <v>A-1005 Kakkad la vida</v>
+        <v>B-903, Kakkad lavida</v>
       </c>
       <c r="E5" t="str">
-        <v>8806022013</v>
+        <v>8109861246</v>
       </c>
       <c r="F5" t="str">
-        <v>Appe Chutney x1, Vermicelli Kheer x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G5">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="H5" t="str">
         <v>DELIVERED</v>
@@ -611,10 +611,10 @@
         <v>2026-01-21</v>
       </c>
       <c r="K5" t="str">
-        <v>18:30</v>
+        <v/>
       </c>
       <c r="L5" t="str">
-        <v>Less spicy</v>
+        <v/>
       </c>
       <c r="M5" t="str">
         <v/>
@@ -625,25 +625,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-20 17:36</v>
+        <v>2026-01-21 07:49</v>
       </c>
       <c r="C6" t="str">
-        <v>Priyanka Patil</v>
+        <v>Renu</v>
       </c>
       <c r="D6" t="str">
-        <v>A-1605</v>
+        <v>A-1005 Kakkad la vida</v>
       </c>
       <c r="E6" t="str">
-        <v>9867003224</v>
+        <v>8806022013</v>
       </c>
       <c r="F6" t="str">
-        <v>Appe Chutney x2</v>
+        <v>Appe Chutney x1, Vermicelli Kheer x1</v>
       </c>
       <c r="G6">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H6" t="str">
         <v>DELIVERED</v>
@@ -655,10 +655,10 @@
         <v>2026-01-21</v>
       </c>
       <c r="K6" t="str">
-        <v>09:15</v>
+        <v>18:30</v>
       </c>
       <c r="L6" t="str">
-        <v/>
+        <v>Less spicy</v>
       </c>
       <c r="M6" t="str">
         <v/>
@@ -669,25 +669,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-20 15:05</v>
+        <v>2026-01-20 17:36</v>
       </c>
       <c r="C7" t="str">
-        <v>Indrani Karmakar</v>
+        <v>Priyanka Patil</v>
       </c>
       <c r="D7" t="str">
-        <v>A-1903</v>
+        <v>A-1605</v>
       </c>
       <c r="E7" t="str">
-        <v>7030961520</v>
+        <v>9867003224</v>
       </c>
       <c r="F7" t="str">
-        <v>Appe Chutney x1</v>
+        <v>Appe Chutney x2</v>
       </c>
       <c r="G7">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="H7" t="str">
         <v>DELIVERED</v>
@@ -699,10 +699,10 @@
         <v>2026-01-21</v>
       </c>
       <c r="K7" t="str">
-        <v>09:00</v>
+        <v>09:15</v>
       </c>
       <c r="L7" t="str">
-        <v>Less spicy. Flavourful</v>
+        <v/>
       </c>
       <c r="M7" t="str">
         <v/>
@@ -713,19 +713,19 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-20 15:03</v>
+        <v>2026-01-20 15:05</v>
       </c>
       <c r="C8" t="str">
-        <v>Udita Roy</v>
+        <v>Indrani Karmakar</v>
       </c>
       <c r="D8" t="str">
-        <v>A-1603</v>
+        <v>A-1903</v>
       </c>
       <c r="E8" t="str">
-        <v>7061856166</v>
+        <v>7030961520</v>
       </c>
       <c r="F8" t="str">
         <v>Appe Chutney x1</v>
@@ -743,7 +743,7 @@
         <v>2026-01-21</v>
       </c>
       <c r="K8" t="str">
-        <v>09:30</v>
+        <v>09:00</v>
       </c>
       <c r="L8" t="str">
         <v>Less spicy. Flavourful</v>
@@ -757,25 +757,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-20 12:17</v>
+        <v>2026-01-20 15:03</v>
       </c>
       <c r="C9" t="str">
-        <v>Radha shelke</v>
+        <v>Udita Roy</v>
       </c>
       <c r="D9" t="str">
-        <v>C 803</v>
+        <v>A-1603</v>
       </c>
       <c r="E9" t="str">
-        <v>9890774770</v>
+        <v>7061856166</v>
       </c>
       <c r="F9" t="str">
-        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Appe Chutney x1</v>
       </c>
       <c r="G9">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H9" t="str">
         <v>DELIVERED</v>
@@ -784,13 +784,13 @@
         <v>PAID</v>
       </c>
       <c r="J9" t="str">
-        <v/>
+        <v>2026-01-21</v>
       </c>
       <c r="K9" t="str">
-        <v/>
+        <v>09:30</v>
       </c>
       <c r="L9" t="str">
-        <v/>
+        <v>Less spicy. Flavourful</v>
       </c>
       <c r="M9" t="str">
         <v/>
@@ -801,25 +801,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-20 11:13</v>
+        <v>2026-01-20 12:17</v>
       </c>
       <c r="C10" t="str">
-        <v>Pooja</v>
+        <v>Radha shelke</v>
       </c>
       <c r="D10" t="str">
-        <v>12</v>
+        <v>C 803</v>
       </c>
       <c r="E10" t="str">
-        <v>9096648553</v>
+        <v>9890774770</v>
       </c>
       <c r="F10" t="str">
-        <v>Til Poli x1</v>
+        <v>Appe Chutney x2, Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="H10" t="str">
         <v>DELIVERED</v>
@@ -828,10 +828,10 @@
         <v>PAID</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-20</v>
+        <v/>
       </c>
       <c r="K10" t="str">
-        <v>16:43</v>
+        <v/>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,25 +845,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-20 05:33</v>
+        <v>2026-01-20 11:13</v>
       </c>
       <c r="C11" t="str">
         <v>Pooja</v>
       </c>
       <c r="D11" t="str">
-        <v>A 1608</v>
+        <v>12</v>
       </c>
       <c r="E11" t="str">
         <v>9096648553</v>
       </c>
       <c r="F11" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H11" t="str">
         <v>DELIVERED</v>
@@ -875,7 +875,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="K11" t="str">
-        <v>11:03</v>
+        <v>16:43</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -889,25 +889,25 @@
     </row>
     <row r="12">
       <c r="A12">
+        <v>21</v>
+      </c>
+      <c r="B12" t="str">
+        <v>2026-01-20 05:33</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D12" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E12" t="str">
+        <v>9096648553</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Jawar Bhakari x1</v>
+      </c>
+      <c r="G12">
         <v>20</v>
-      </c>
-      <c r="B12" t="str">
-        <v>2026-01-20 01:42</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Minakshi</v>
-      </c>
-      <c r="D12" t="str">
-        <v>A 201</v>
-      </c>
-      <c r="E12" t="str">
-        <v>7387851735</v>
-      </c>
-      <c r="F12" t="str">
-        <v>Wheat Chapati x2</v>
-      </c>
-      <c r="G12">
-        <v>30</v>
       </c>
       <c r="H12" t="str">
         <v>DELIVERED</v>
@@ -919,7 +919,7 @@
         <v>2026-01-20</v>
       </c>
       <c r="K12" t="str">
-        <v>08:00</v>
+        <v>11:03</v>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -933,25 +933,25 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="str">
-        <v>2026-01-19 09:18</v>
+        <v>2026-01-20 01:42</v>
       </c>
       <c r="C13" t="str">
-        <v>Surekha Sonawane</v>
+        <v>Minakshi</v>
       </c>
       <c r="D13" t="str">
-        <v>A 808</v>
+        <v>A 201</v>
       </c>
       <c r="E13" t="str">
-        <v>935917349</v>
+        <v>7387851735</v>
       </c>
       <c r="F13" t="str">
-        <v>Til Poli x4</v>
+        <v>Wheat Chapati x2</v>
       </c>
       <c r="G13">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="H13" t="str">
         <v>DELIVERED</v>
@@ -960,10 +960,10 @@
         <v>PAID</v>
       </c>
       <c r="J13" t="str">
-        <v>2026-01-18</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K13" t="str">
-        <v>16:00</v>
+        <v>08:00</v>
       </c>
       <c r="L13" t="str">
         <v/>
@@ -977,22 +977,22 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" t="str">
-        <v>2026-01-19 08:37</v>
+        <v>2026-01-19 09:18</v>
       </c>
       <c r="C14" t="str">
-        <v>Radhika Joshi</v>
+        <v>Surekha Sonawane</v>
       </c>
       <c r="D14" t="str">
-        <v>C 1501</v>
+        <v>A 808</v>
       </c>
       <c r="E14" t="str">
-        <v>9967195227</v>
+        <v>935917349</v>
       </c>
       <c r="F14" t="str">
-        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
+        <v>Til Poli x4</v>
       </c>
       <c r="G14">
         <v>120</v>
@@ -1004,10 +1004,10 @@
         <v>PAID</v>
       </c>
       <c r="J14" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-18</v>
       </c>
       <c r="K14" t="str">
-        <v>08:00</v>
+        <v>16:00</v>
       </c>
       <c r="L14" t="str">
         <v/>
@@ -1021,25 +1021,25 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" t="str">
-        <v>2026-01-19 05:42</v>
+        <v>2026-01-19 08:37</v>
       </c>
       <c r="C15" t="str">
-        <v>Prajakta Patil</v>
+        <v>Radhika Joshi</v>
       </c>
       <c r="D15" t="str">
-        <v>A 804</v>
+        <v>C 1501</v>
       </c>
       <c r="E15" t="str">
-        <v>779868817</v>
+        <v>9967195227</v>
       </c>
       <c r="F15" t="str">
-        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
+        <v>Pohe x2, Wheat Chapati x2, Upma x1</v>
       </c>
       <c r="G15">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="H15" t="str">
         <v>DELIVERED</v>
@@ -1048,7 +1048,7 @@
         <v>PAID</v>
       </c>
       <c r="J15" t="str">
-        <v>2026-01-22</v>
+        <v>2026-01-20</v>
       </c>
       <c r="K15" t="str">
         <v>08:00</v>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="str">
-        <v>2026-01-19 05:41</v>
+        <v>2026-01-19 05:42</v>
       </c>
       <c r="C16" t="str">
         <v>Prajakta Patil</v>
@@ -1080,10 +1080,10 @@
         <v>779868817</v>
       </c>
       <c r="F16" t="str">
-        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+        <v>Wheat Chapati x3, 1 Plate Bhaji x1</v>
       </c>
       <c r="G16">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="H16" t="str">
         <v>DELIVERED</v>
@@ -1092,7 +1092,7 @@
         <v>PAID</v>
       </c>
       <c r="J16" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-22</v>
       </c>
       <c r="K16" t="str">
         <v>08:00</v>
@@ -1109,10 +1109,10 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="str">
-        <v>2026-01-19 05:39</v>
+        <v>2026-01-19 05:41</v>
       </c>
       <c r="C17" t="str">
         <v>Prajakta Patil</v>
@@ -1136,13 +1136,13 @@
         <v>PAID</v>
       </c>
       <c r="J17" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="K17" t="str">
         <v>08:00</v>
       </c>
       <c r="L17" t="str">
-        <v>Less Spicy</v>
+        <v/>
       </c>
       <c r="M17" t="str">
         <v/>
@@ -1153,58 +1153,102 @@
     </row>
     <row r="18">
       <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="str">
+        <v>2026-01-19 05:39</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Prajakta Patil</v>
+      </c>
+      <c r="D18" t="str">
+        <v>A 804</v>
+      </c>
+      <c r="E18" t="str">
+        <v>779868817</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Wheat Chapati x5, 1 Plate Bhaji x1</v>
+      </c>
+      <c r="G18">
+        <v>105</v>
+      </c>
+      <c r="H18" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I18" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J18" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="K18" t="str">
+        <v>08:00</v>
+      </c>
+      <c r="L18" t="str">
+        <v>Less Spicy</v>
+      </c>
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
         <v>14</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B19" t="str">
         <v>2026-01-14 17:08</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C19" t="str">
         <v>Mrunal</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D19" t="str">
         <v>KLV B 2108</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E19" t="str">
         <v>9404665203</v>
       </c>
-      <c r="F18" t="str">
+      <c r="F19" t="str">
         <v>Wheat Chapati x40</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>600</v>
       </c>
-      <c r="H18" t="str">
-        <v>DELIVERED</v>
-      </c>
-      <c r="I18" t="str">
-        <v>PAID</v>
-      </c>
-      <c r="J18" t="str">
+      <c r="H19" t="str">
+        <v>DELIVERED</v>
+      </c>
+      <c r="I19" t="str">
+        <v>PAID</v>
+      </c>
+      <c r="J19" t="str">
         <v>2026-01-15</v>
       </c>
-      <c r="K18" t="str">
+      <c r="K19" t="str">
         <v>00:30</v>
       </c>
-      <c r="L18" t="str">
-        <v/>
-      </c>
-      <c r="M18" t="str">
-        <v/>
-      </c>
-      <c r="N18" t="str">
+      <c r="L19" t="str">
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N19"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1234,68 +1278,68 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-27</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F2">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2026-01-21</v>
+        <v>2026-01-26</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>170</v>
+        <v>115</v>
       </c>
       <c r="F3">
-        <v>170</v>
+        <v>75</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2026-01-20</v>
+        <v>2026-01-21</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>500</v>
+        <v>170</v>
       </c>
       <c r="F4">
-        <v>500</v>
+        <v>170</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1303,22 +1347,22 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2026-01-19</v>
+        <v>2026-01-20</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>525</v>
+        <v>500</v>
       </c>
       <c r="F5">
-        <v>525</v>
+        <v>500</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1326,30 +1370,53 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-19</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>600</v>
+        <v>525</v>
       </c>
       <c r="F6">
-        <v>600</v>
+        <v>525</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2026-01-14</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>600</v>
+      </c>
+      <c r="F7">
+        <v>600</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-27.xlsx - 2026-01-27T14:10:19.345Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-27.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-27.xlsx
@@ -470,7 +470,7 @@
         <v>80</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -1284,7 +1284,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-27.xlsx - 2026-01-27T14:10:38.664Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-27.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-27.xlsx
@@ -558,7 +558,7 @@
         <v>40</v>
       </c>
       <c r="H4" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
@@ -1307,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>